<commit_message>
Cyclic output of text information using the Stream API
</commit_message>
<xml_diff>
--- a/src/main/resources/universityInfo.xlsx
+++ b/src/main/resources/universityInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Флешка\Перенос на новый комп\idea\.gradle\module_gradle\universitet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53C63B3-27A2-4AB1-BF65-5E04AD3B7C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1779DDA9-C74E-4A17-8F1C-0F0A12A5D799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="18900" windowHeight="11770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Студенты" sheetId="1" r:id="rId1"/>
@@ -123,40 +123,40 @@
     <t>Средний балл</t>
   </si>
   <si>
+    <t>Козлов М. В.</t>
+  </si>
+  <si>
+    <t>Фёдоров А. И.</t>
+  </si>
+  <si>
+    <t>Игнатьев М. М.</t>
+  </si>
+  <si>
+    <t>Соколов В. В.</t>
+  </si>
+  <si>
+    <t>Сидоров Е. Г.</t>
+  </si>
+  <si>
+    <t>Витальев В. А.</t>
+  </si>
+  <si>
+    <t>Петров П. А.</t>
+  </si>
+  <si>
+    <t>Алексеев С. В.</t>
+  </si>
+  <si>
+    <t>Иванов А. Г.</t>
+  </si>
+  <si>
+    <t>Васильев В. П.</t>
+  </si>
+  <si>
+    <t>0020-high</t>
+  </si>
+  <si>
     <t>Иванов И. А.</t>
-  </si>
-  <si>
-    <t>Козлов М. В.</t>
-  </si>
-  <si>
-    <t>Фёдоров А. И.</t>
-  </si>
-  <si>
-    <t>Игнатьев М. М.</t>
-  </si>
-  <si>
-    <t>Соколов В. В.</t>
-  </si>
-  <si>
-    <t>Сидоров Е. Г.</t>
-  </si>
-  <si>
-    <t>Витальев В. А.</t>
-  </si>
-  <si>
-    <t>Петров П. А.</t>
-  </si>
-  <si>
-    <t>Алексеев С. В.</t>
-  </si>
-  <si>
-    <t>Иванов А. Г.</t>
-  </si>
-  <si>
-    <t>Васильев В. П.</t>
-  </si>
-  <si>
-    <t>MEDICINA</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,7 +577,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
@@ -591,7 +591,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -605,7 +605,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
@@ -619,7 +619,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
@@ -633,7 +633,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -647,7 +647,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3">
         <v>2</v>
@@ -661,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3">
         <v>2</v>
@@ -675,7 +675,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -689,7 +689,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -703,7 +703,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3">
         <v>3</v>
@@ -717,7 +717,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3">
         <v>4</v>
@@ -736,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -786,7 +786,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -832,7 +832,7 @@
         <v>1995</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Create and populate a new Excel file with Apache POI, work with table styles, collect statistics using the Java Stream API, use BigDecimal to convert numbers
</commit_message>
<xml_diff>
--- a/src/main/resources/universityInfo.xlsx
+++ b/src/main/resources/universityInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Флешка\Перенос на новый комп\idea\.gradle\module_gradle\universitet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1779DDA9-C74E-4A17-8F1C-0F0A12A5D799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212AC38C-A564-4508-B392-5D1088B870D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="18900" windowHeight="11770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Студенты" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>id университета</t>
   </si>
@@ -123,6 +123,9 @@
     <t>Средний балл</t>
   </si>
   <si>
+    <t>Иванов И. А.</t>
+  </si>
+  <si>
     <t>Козлов М. В.</t>
   </si>
   <si>
@@ -151,12 +154,6 @@
   </si>
   <si>
     <t>Васильев В. П.</t>
-  </si>
-  <si>
-    <t>0020-high</t>
-  </si>
-  <si>
-    <t>Иванов И. А.</t>
   </si>
 </sst>
 </file>
@@ -202,11 +199,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -548,14 +546,15 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -568,7 +567,7 @@
       <c r="C1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -577,7 +576,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
@@ -591,7 +590,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -605,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
@@ -619,7 +618,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
@@ -633,13 +632,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>4.8499999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -647,7 +646,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="3">
         <v>2</v>
@@ -661,13 +660,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3">
         <v>2</v>
       </c>
       <c r="D8" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -675,7 +674,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -689,13 +688,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -703,13 +702,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3">
         <v>3</v>
       </c>
       <c r="D11" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -717,13 +716,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="3">
         <v>4</v>
       </c>
       <c r="D12" s="3">
-        <v>4.7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +736,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -786,7 +785,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>

</xml_diff>